<commit_message>
New test file (from MagicBox) Fixed a format error in the former New test file Fixed bug due to None value when updating categories in a taxonomy
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_1.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -467,13 +467,14 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,21 +615,23 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="64.0510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="71.9693877551021"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="63.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="71.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,13 +1788,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,15 +2060,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>